<commit_message>
07.07.2020 MC Sales Details
</commit_message>
<xml_diff>
--- a/2020/July/All Details/06.07.2020/MC Balance Transfer July 2020.xlsx
+++ b/2020/July/All Details/06.07.2020/MC Balance Transfer July 2020.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="103">
   <si>
     <t>Date</t>
   </si>
@@ -328,6 +328,9 @@
   </si>
   <si>
     <t>06.07.2020</t>
+  </si>
+  <si>
+    <t>Haider</t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1150,7 @@
         <xdr:cNvPr id="1317" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEF7B42F-C37B-44F8-8D5A-2ED7FEE15E8A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1159,7 +1162,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -1182,14 +1185,14 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1497,9 +1500,9 @@
   <dimension ref="A1:BI231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="I1" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="E95" sqref="E95"/>
+      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -2091,14 +2094,14 @@
         <v>512450</v>
       </c>
       <c r="C9" s="2">
-        <v>520725</v>
+        <v>519725</v>
       </c>
       <c r="D9" s="2">
         <v>5200</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>525925</v>
+        <v>524925</v>
       </c>
       <c r="F9" s="96"/>
       <c r="G9" s="17"/>
@@ -3731,7 +3734,7 @@
       </c>
       <c r="C33" s="2">
         <f>SUM(C5:C32)</f>
-        <v>2258295</v>
+        <v>2257295</v>
       </c>
       <c r="D33" s="2">
         <f>SUM(D5:D32)</f>
@@ -3739,11 +3742,11 @@
       </c>
       <c r="E33" s="2">
         <f>SUM(E5:E32)</f>
-        <v>2266725</v>
+        <v>2265725</v>
       </c>
       <c r="F33" s="67">
         <f>B33-E33</f>
-        <v>-434885</v>
+        <v>-433885</v>
       </c>
       <c r="G33" s="81"/>
       <c r="H33" s="86"/>
@@ -4291,10 +4294,18 @@
       <c r="BI40" s="7"/>
     </row>
     <row r="41" spans="1:61" ht="12.6" customHeight="1">
-      <c r="A41" s="123"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="1"/>
+      <c r="A41" s="123" t="s">
+        <v>102</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>101</v>
+      </c>
       <c r="E41" s="18"/>
       <c r="F41" s="95"/>
       <c r="G41" s="83"/>
@@ -8503,7 +8514,7 @@
       <c r="B98" s="145"/>
       <c r="C98" s="32">
         <f>SUM(C37:C97)</f>
-        <v>1637778</v>
+        <v>1638778</v>
       </c>
       <c r="D98" s="28"/>
       <c r="F98" s="110"/>
@@ -8658,7 +8669,7 @@
       <c r="B100" s="143"/>
       <c r="C100" s="29">
         <f>C98+L121</f>
-        <v>1637778</v>
+        <v>1638778</v>
       </c>
       <c r="D100" s="21"/>
       <c r="F100" s="48"/>

</xml_diff>